<commit_message>
fix: sua loi trich dan nguon hien n/a
</commit_message>
<xml_diff>
--- a/quizzes/10. Kiểm tra giám sát nội bộ.xlsx
+++ b/quizzes/10. Kiểm tra giám sát nội bộ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uybinh/Projects/quiz-nghiep-vu/quizzes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F1CB14-8120-D347-A5F8-CDB9FE76BFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28B9D1B-55F1-3A4A-8591-FCC1FE697D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="32000" windowHeight="18080" tabRatio="789" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="1430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="1431">
   <si>
     <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM
 Độc lập - Tự do - Hạnh phúc</t>
@@ -4580,6 +4580,9 @@
   </si>
   <si>
     <t>ĐÁP ÁN 4</t>
+  </si>
+  <si>
+    <t>TRÍCH DẪN NGUỒN</t>
   </si>
 </sst>
 </file>
@@ -7331,7 +7334,7 @@
   <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -7371,7 +7374,7 @@
         <v>1421</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>8</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: sua loi trich dan nguon hien n/a (#65)
</commit_message>
<xml_diff>
--- a/quizzes/10. Kiểm tra giám sát nội bộ.xlsx
+++ b/quizzes/10. Kiểm tra giám sát nội bộ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uybinh/Projects/quiz-nghiep-vu/quizzes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F1CB14-8120-D347-A5F8-CDB9FE76BFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28B9D1B-55F1-3A4A-8591-FCC1FE697D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="32000" windowHeight="18080" tabRatio="789" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="1430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="1431">
   <si>
     <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM
 Độc lập - Tự do - Hạnh phúc</t>
@@ -4580,6 +4580,9 @@
   </si>
   <si>
     <t>ĐÁP ÁN 4</t>
+  </si>
+  <si>
+    <t>TRÍCH DẪN NGUỒN</t>
   </si>
 </sst>
 </file>
@@ -7331,7 +7334,7 @@
   <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -7371,7 +7374,7 @@
         <v>1421</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>8</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.2">

</xml_diff>